<commit_message>
Updated pom to read testng.xml for test runs
</commit_message>
<xml_diff>
--- a/src/test/resources/flipkart_test_cases.xlsx
+++ b/src/test/resources/flipkart_test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashgupta02\eclipse-qa\exit-test-automation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nagarro-my.sharepoint.com/personal/yash_gupta02_nagarro_com/Documents/Desktop/github Projects/exit-test-automation/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F032F4-1770-4A47-A595-A00F27FA8201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{16F032F4-1770-4A47-A595-A00F27FA8201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27CFB81C-9304-4987-AE97-48676E2F0ED9}"/>
   <bookViews>
     <workbookView xWindow="1416" yWindow="1332" windowWidth="19788" windowHeight="9852" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,7 +706,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F3" sqref="F3:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +806,7 @@
         <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>60</v>
@@ -829,7 +829,7 @@
         <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
         <v>63</v>
@@ -852,7 +852,7 @@
         <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
         <v>61</v>
@@ -875,7 +875,7 @@
         <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
         <v>70</v>
@@ -898,7 +898,7 @@
         <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
         <v>71</v>
@@ -921,7 +921,7 @@
         <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
         <v>72</v>
@@ -944,7 +944,7 @@
         <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>59</v>
@@ -967,7 +967,7 @@
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
         <v>73</v>
@@ -990,7 +990,7 @@
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>74</v>
@@ -1013,7 +1013,7 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
         <v>75</v>
@@ -1036,7 +1036,7 @@
         <v>20000</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
         <v>78</v>
@@ -1059,7 +1059,7 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
         <v>79</v>
@@ -1082,7 +1082,7 @@
         <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G16" t="s">
         <v>80</v>
@@ -1105,7 +1105,7 @@
         <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
         <v>90</v>
@@ -1128,7 +1128,7 @@
         <v>84</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
         <v>85</v>
@@ -1151,7 +1151,7 @@
         <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
         <v>89</v>
@@ -1174,7 +1174,7 @@
         <v>99</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G20" t="s">
         <v>93</v>
@@ -1197,7 +1197,7 @@
         <v>7881132091</v>
       </c>
       <c r="F21" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="G21" t="s">
         <v>98</v>

</xml_diff>